<commit_message>
Final coding start debage
</commit_message>
<xml_diff>
--- a/InputData.xlsx
+++ b/InputData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
   <si>
     <t>S</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r </t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1020,7 @@
   <dimension ref="A1:DQ18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CR1" workbookViewId="0">
-      <selection activeCell="DQ3" sqref="DQ3"/>
+      <selection activeCell="CY1" sqref="CY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1312,7 +1315,7 @@
       </c>
       <c r="CX1" s="3"/>
       <c r="CY1" s="2" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="DA1" s="2" t="s">
         <v>75</v>

</xml_diff>